<commit_message>
dw: new tape added
</commit_message>
<xml_diff>
--- a/v2/public/data/FMA Media List.xlsx
+++ b/v2/public/data/FMA Media List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cassettes" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
   <si>
     <t>ID</t>
   </si>
@@ -1400,6 +1400,12 @@
   </si>
   <si>
     <t xml:space="preserve">Hard Drone / Soft Drone / Brad / Bleeps cars voices</t>
+  </si>
+  <si>
+    <t>FMACM14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JB Pat Multi</t>
   </si>
   <si>
     <t xml:space="preserve">Source Format</t>
@@ -2028,7 +2034,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView topLeftCell="I5" zoomScale="64" workbookViewId="0">
-      <selection activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection activeCell="C103" activeCellId="0" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="12"/>
@@ -6201,10 +6207,10 @@
   </sheetPr>
   <sheetViews>
     <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="32" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="32" defaultRowHeight="12"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="15.738300000000001"/>
     <col customWidth="1" min="2" max="2" style="1" width="19.503900000000002"/>
@@ -6219,7 +6225,7 @@
     <col customWidth="1" min="11" max="257" style="1" width="32.828099999999999"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1" s="1" customFormat="1" ht="13.1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6270,7 +6276,7 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
     </row>
-    <row r="2" s="1" customFormat="1">
+    <row r="2" s="1" customFormat="1" ht="13.1">
       <c r="A2" s="1" t="s">
         <v>409</v>
       </c>
@@ -6297,7 +6303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1">
+    <row r="3" s="1" customFormat="1" ht="13.1">
       <c r="A3" s="1" t="s">
         <v>414</v>
       </c>
@@ -6324,7 +6330,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1">
+    <row r="4" s="1" customFormat="1" ht="13.1">
       <c r="A4" s="1" t="s">
         <v>419</v>
       </c>
@@ -6356,7 +6362,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1">
+    <row r="5" s="1" customFormat="1" ht="13.1">
       <c r="A5" s="1" t="s">
         <v>424</v>
       </c>
@@ -6386,7 +6392,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1">
+    <row r="6" s="1" customFormat="1" ht="13.1">
       <c r="A6" s="1" t="s">
         <v>429</v>
       </c>
@@ -6416,7 +6422,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1">
+    <row r="7" s="1" customFormat="1" ht="13.1">
       <c r="A7" s="1" t="s">
         <v>433</v>
       </c>
@@ -6448,7 +6454,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1">
+    <row r="8" s="1" customFormat="1" ht="13.1">
       <c r="A8" s="1" t="s">
         <v>436</v>
       </c>
@@ -6476,7 +6482,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1">
+    <row r="9" s="1" customFormat="1" ht="13.1">
       <c r="A9" s="1" t="s">
         <v>440</v>
       </c>
@@ -6503,7 +6509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1">
+    <row r="10" s="1" customFormat="1" ht="13.1">
       <c r="A10" s="1" t="s">
         <v>443</v>
       </c>
@@ -6533,7 +6539,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1">
+    <row r="11" s="1" customFormat="1" ht="13.1">
       <c r="A11" s="1" t="s">
         <v>447</v>
       </c>
@@ -6562,7 +6568,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1">
+    <row r="12" s="1" customFormat="1" ht="13.1">
       <c r="A12" s="1" t="s">
         <v>452</v>
       </c>
@@ -6588,7 +6594,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" ht="12.75">
+    <row r="13" ht="13.1">
       <c r="A13" s="1" t="s">
         <v>455</v>
       </c>
@@ -6602,15 +6608,15 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" ht="12.75">
+    <row r="14" ht="13.1">
       <c r="A14" s="1" t="s">
         <v>457</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>448</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>411</v>
@@ -6623,6 +6629,23 @@
       </c>
       <c r="H14" s="1" t="s">
         <v>459</v>
+      </c>
+    </row>
+    <row r="15" ht="13.1">
+      <c r="A15" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -6666,7 +6689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -6711,16 +6734,16 @@
     </row>
     <row r="2" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>98</v>
@@ -6729,7 +6752,7 @@
         <v>170</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="H2" s="2">
         <v>34486</v>
@@ -6737,59 +6760,59 @@
     </row>
     <row r="3" ht="12.75">
       <c r="A3" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="A4" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>406</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="A5" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>98</v>
@@ -6798,7 +6821,7 @@
         <v>406</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="H5" s="2">
         <v>38193</v>
@@ -6806,33 +6829,33 @@
     </row>
     <row r="6" ht="12.75">
       <c r="A6" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>285</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="A7" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -6841,13 +6864,13 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="H7" s="2">
         <v>1990</v>
@@ -6855,10 +6878,10 @@
     </row>
     <row r="8" ht="12.75">
       <c r="A8" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -6867,21 +6890,21 @@
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" ht="12.75">
       <c r="A9" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -6890,16 +6913,16 @@
         <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>